<commit_message>
Modification des données supprimées
</commit_message>
<xml_diff>
--- a/data/data_correction/DataCorrigée.xlsx
+++ b/data/data_correction/DataCorrigée.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eye-tracking\Simulateddata\data_correction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eye-tracking\Simulateddata\data\data_correction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1593B34-EF6C-441E-950F-960F1ED265AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D1E846-0947-46F0-91AB-3009ED96FF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B1FCA952-E8D3-4689-8AF6-C925CC51F46F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B1FCA952-E8D3-4689-8AF6-C925CC51F46F}"/>
   </bookViews>
   <sheets>
     <sheet name="Coord" sheetId="5" r:id="rId1"/>
@@ -501,8 +501,8 @@
   <sheetPr codeName="Feuil4"/>
   <dimension ref="A1:J433"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I115" sqref="I115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9711,7 +9711,7 @@
   <dimension ref="A1:F433"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E99" sqref="E99"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15803,10 +15803,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CB1D53-6E59-481E-99C7-4CA3A42011D4}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16032,7 +16032,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="5">
-        <v>672</v>
+        <v>327</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -16040,7 +16040,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5">
-        <v>756</v>
+        <v>672</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -16048,14 +16048,22 @@
         <v>40</v>
       </c>
       <c r="B29" s="5">
-        <v>980</v>
+        <v>756</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
+        <v>40</v>
+      </c>
+      <c r="B30" s="5">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
         <v>47</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B31" s="5">
         <v>980</v>
       </c>
     </row>

</xml_diff>